<commit_message>
added the remaining excel samples
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -59,9 +59,6 @@
     <t>failed</t>
   </si>
   <si>
-    <t>new user</t>
-  </si>
-  <si>
     <t>avg</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>update shit</t>
+  </si>
+  <si>
+    <t>newasdasd user</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,10 +418,10 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -429,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>